<commit_message>
Updated Edit Product Details script
</commit_message>
<xml_diff>
--- a/tests/artifact/data/EditProductDetails.data.xlsx
+++ b/tests/artifact/data/EditProductDetails.data.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="423">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="425">
   <si>
     <t>login.screen</t>
   </si>
@@ -937,7 +937,13 @@
     <t>Back.Button</t>
   </si>
   <si>
+    <t>//button[@class="btn m-1 btn-danger btn-sm"]</t>
+  </si>
+  <si>
     <t>Reset.Button</t>
+  </si>
+  <si>
+    <t>//button[@class="btn m-1 btn-warning btn-sm"]</t>
   </si>
   <si>
     <t>Save.Button</t>
@@ -2436,8 +2442,8 @@
   <sheetPr/>
   <dimension ref="A1:XFD284"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="125" topLeftCell="B129" workbookViewId="0">
-      <selection activeCell="B129" sqref="B129"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="125" topLeftCell="B160" workbookViewId="0">
+      <selection activeCell="B185" sqref="B185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7" defaultRowHeight="16"/>
@@ -69448,20 +69454,20 @@
         <v>299</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>69</v>
+        <v>300</v>
       </c>
     </row>
     <row r="185" spans="1:2">
       <c r="A185" s="4" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>71</v>
+        <v>302</v>
       </c>
     </row>
     <row r="186" spans="1:2">
       <c r="A186" s="4" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="B186" s="2" t="s">
         <v>73</v>
@@ -69469,7 +69475,7 @@
     </row>
     <row r="187" spans="1:2">
       <c r="A187" s="4" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="B187" s="2" t="s">
         <v>75</v>
@@ -69731,7 +69737,7 @@
         <v>127</v>
       </c>
       <c r="B219" s="2" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
     </row>
     <row r="220" spans="1:2">
@@ -69752,10 +69758,10 @@
     </row>
     <row r="222" spans="1:2">
       <c r="A222" s="4" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="B222" s="2" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
     <row r="223" spans="1:2">
@@ -69768,58 +69774,58 @@
     </row>
     <row r="224" spans="1:2">
       <c r="A224" s="1" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="B224" s="2" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
     </row>
     <row r="225" spans="1:2">
       <c r="A225" s="1" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="B225" s="2" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
     </row>
     <row r="226" spans="1:2">
       <c r="A226" s="1" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="B226" s="2" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
     </row>
     <row r="227" spans="1:2">
       <c r="A227" s="1" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="B227" s="2" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
     </row>
     <row r="228" spans="1:2">
       <c r="A228" s="1" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="B228" s="2" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
     </row>
     <row r="229" spans="1:2">
       <c r="A229" s="1" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="B229" s="2" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
     </row>
     <row r="230" spans="1:2">
       <c r="A230" s="1" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="B230" s="2" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
     </row>
     <row r="231" spans="1:2">
@@ -69832,415 +69838,415 @@
     </row>
     <row r="232" spans="1:2">
       <c r="A232" s="1" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="B232" s="2" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
     </row>
     <row r="233" spans="1:2">
       <c r="A233" s="1" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="B233" s="2" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
     </row>
     <row r="234" spans="1:2">
       <c r="A234" s="1" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="B234" s="2" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
     </row>
     <row r="235" spans="1:2">
       <c r="A235" s="1" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="B235" s="2" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
     </row>
     <row r="236" spans="1:2">
       <c r="A236" s="1" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="B236" s="2" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
     </row>
     <row r="237" spans="1:2">
       <c r="A237" s="1" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="B237" s="2" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
     </row>
     <row r="238" spans="1:2">
       <c r="A238" s="1" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="B238" s="2" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row r="239" spans="1:2">
       <c r="A239" s="1" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="B239" s="2" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
     </row>
     <row r="240" spans="1:2">
       <c r="A240" s="1" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="B240" s="2" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
     </row>
     <row r="241" spans="1:2">
       <c r="A241" s="1" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="B241" s="2" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
     </row>
     <row r="242" spans="1:2">
       <c r="A242" s="1" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="B242" s="2" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
     </row>
     <row r="243" spans="1:2">
       <c r="A243" s="1" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="B243" s="2" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
     </row>
     <row r="244" spans="1:2">
       <c r="A244" s="1" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="B244" s="2" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
     </row>
     <row r="245" spans="1:2">
       <c r="A245" s="1" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="B245" s="2" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
     </row>
     <row r="246" spans="1:2">
       <c r="A246" s="1" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="B246" s="2" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
     </row>
     <row r="247" spans="1:2">
       <c r="A247" s="1" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="B247" s="2" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
     </row>
     <row r="248" spans="1:2">
       <c r="A248" s="1" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="B248" s="2" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
     </row>
     <row r="249" spans="1:2">
       <c r="A249" s="1" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="B249" s="2" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
     </row>
     <row r="250" spans="1:2">
       <c r="A250" s="1" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="B250" s="2" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
     </row>
     <row r="251" spans="1:2">
       <c r="A251" s="1" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="B251" s="2" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
     </row>
     <row r="252" spans="1:2">
       <c r="A252" s="1" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="B252" s="2" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
     </row>
     <row r="253" spans="1:2">
       <c r="A253" s="1" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="B253" s="2" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
     </row>
     <row r="254" spans="1:2">
       <c r="A254" s="1" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="B254" s="2" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="255" spans="1:2">
       <c r="A255" s="1" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="B255" s="2" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
     </row>
     <row r="256" spans="1:2">
       <c r="A256" s="1" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="B256" s="2" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
     </row>
     <row r="257" spans="1:2">
       <c r="A257" s="1" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="B257" s="2" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
     </row>
     <row r="258" spans="1:2">
       <c r="A258" s="1" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="B258" s="2" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
     </row>
     <row r="259" spans="1:2">
       <c r="A259" s="1" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="B259" s="2" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
     </row>
     <row r="260" spans="1:2">
       <c r="A260" s="1" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="B260" s="2" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
     </row>
     <row r="261" spans="1:2">
       <c r="A261" s="1" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="B261" s="2" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
     </row>
     <row r="262" spans="1:2">
       <c r="A262" s="1" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="B262" s="2" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
     </row>
     <row r="263" spans="1:2">
       <c r="A263" s="1" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="B263" s="2" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
     </row>
     <row r="264" spans="1:2">
       <c r="A264" s="1" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="B264" s="2" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
     </row>
     <row r="265" spans="1:2">
       <c r="A265" s="1" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="B265" s="2" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
     </row>
     <row r="266" spans="1:2">
       <c r="A266" s="1" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="B266" s="2" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
     </row>
     <row r="267" spans="1:2">
       <c r="A267" s="1" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="B267" s="2" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
     </row>
     <row r="268" spans="1:2">
       <c r="A268" s="1" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="B268" s="2" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
     </row>
     <row r="269" spans="1:2">
       <c r="A269" s="1" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="B269" s="2" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
     </row>
     <row r="270" spans="1:2">
       <c r="A270" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="B270" s="2" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
     </row>
     <row r="271" spans="1:2">
       <c r="A271" s="1" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="B271" s="2" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
     </row>
     <row r="272" spans="1:2">
       <c r="A272" s="1" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="B272" s="2" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
     </row>
     <row r="273" spans="1:2">
       <c r="A273" s="1" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="B273" s="2" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
     </row>
     <row r="274" spans="1:2">
       <c r="A274" s="1" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="B274" s="2" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
     </row>
     <row r="275" spans="1:2">
       <c r="A275" s="1" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="B275" s="2" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
     </row>
     <row r="276" spans="1:2">
       <c r="A276" s="1" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="B276" s="2" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
     </row>
     <row r="277" spans="1:2">
       <c r="A277" s="1" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="B277" s="2" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
     </row>
     <row r="278" spans="1:2">
       <c r="A278" s="1" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="B278" s="2" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
     </row>
     <row r="279" spans="1:2">
       <c r="A279" s="1" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="B279" s="2" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
     </row>
     <row r="280" spans="1:2">
       <c r="A280" s="1" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="B280" s="2" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
     </row>
     <row r="281" spans="1:2">
       <c r="A281" s="1" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="B281" s="2" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
     </row>
     <row r="282" spans="1:2">
       <c r="A282" s="1" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="B282" s="2" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
     </row>
     <row r="283" spans="1:2">
       <c r="A283" s="1" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="B283" s="2" t="s">
         <v>201</v>
@@ -70248,7 +70254,7 @@
     </row>
     <row r="284" spans="2:2">
       <c r="B284" s="2" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
     </row>
   </sheetData>

</xml_diff>